<commit_message>
Updated flash part number to that actually used: Macronix MX25L6445E. Propagated to schematic and BOM.
</commit_message>
<xml_diff>
--- a/Manufacturing/Swallow-V2/bom/Swallow-V2-BOM.xlsx
+++ b/Manufacturing/Swallow-V2/bom/Swallow-V2-BOM.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1990" uniqueCount="644">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1989" uniqueCount="642">
   <si>
     <t>XMP16-V2 BOM</t>
   </si>
@@ -1795,19 +1795,13 @@
     <t>U57</t>
   </si>
   <si>
-    <t>S25FL064K</t>
+    <t>MX25L6445E</t>
   </si>
   <si>
     <t>SOC088 Wide</t>
   </si>
   <si>
-    <t>Spansion</t>
-  </si>
-  <si>
-    <t>S25FL064K0SMFI011</t>
-  </si>
-  <si>
-    <t>http://uk.farnell.com/spansion/s25fl064k0smfi011/memory-flash-64m-3v-spi-8soic/dp/1861631?Ntt=S25FL064K</t>
+    <t>Macronix</t>
   </si>
   <si>
     <t>U58</t>
@@ -2258,19 +2252,19 @@
   </sheetPr>
   <dimension ref="A1:F400"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="B188" view="normal" windowProtection="false" workbookViewId="0" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="100">
-      <selection activeCell="E189" activeCellId="0" pane="topLeft" sqref="E189"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A347" view="normal" windowProtection="false" workbookViewId="0" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="100">
+      <selection activeCell="B371" activeCellId="0" pane="topLeft" sqref="B371"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.2078431372549"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.6274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.3725490196078"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.6901960784314"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="5.22745098039216"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.7450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="18.4509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.8196078431373"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="1">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2279,31 +2273,31 @@
         <v>41127</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="2">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="2">
       <c r="E2" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="3">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="3">
       <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="4">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="4">
       <c r="B4" s="4"/>
       <c r="E4" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="5">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="5">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="3"/>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="6">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="6">
       <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="9">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="A9" s="0" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +2357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.95" outlineLevel="0" r="12">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="12">
       <c r="A12" s="0" t="s">
         <v>22</v>
       </c>
@@ -5363,7 +5357,7 @@
         <v>234</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="162">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="162">
       <c r="A162" s="5" t="s">
         <v>249</v>
       </c>
@@ -5374,7 +5368,7 @@
         <v>251</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="163">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="163">
       <c r="A163" s="5" t="s">
         <v>252</v>
       </c>
@@ -5385,7 +5379,7 @@
         <v>251</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="164">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="164">
       <c r="A164" s="5" t="s">
         <v>253</v>
       </c>
@@ -5396,7 +5390,7 @@
         <v>251</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="165">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="165">
       <c r="A165" s="5" t="s">
         <v>254</v>
       </c>
@@ -5407,7 +5401,7 @@
         <v>251</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="166">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="166">
       <c r="A166" s="5" t="s">
         <v>255</v>
       </c>
@@ -5418,7 +5412,7 @@
         <v>251</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="167">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="167">
       <c r="A167" s="5" t="s">
         <v>256</v>
       </c>
@@ -5789,7 +5783,7 @@
         <v>281</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="186">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="186">
       <c r="A186" s="0" t="s">
         <v>297</v>
       </c>
@@ -5800,7 +5794,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="187">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="187">
       <c r="A187" s="0" t="s">
         <v>300</v>
       </c>
@@ -5811,7 +5805,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="188">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="188">
       <c r="A188" s="0" t="s">
         <v>302</v>
       </c>
@@ -5822,7 +5816,7 @@
         <v>304</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.45" outlineLevel="0" r="189">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="189">
       <c r="A189" s="0" t="s">
         <v>305</v>
       </c>
@@ -5842,7 +5836,7 @@
         <v>308</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="190">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="190">
       <c r="A190" s="0" t="s">
         <v>309</v>
       </c>
@@ -5853,7 +5847,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="191">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="191">
       <c r="A191" s="0" t="s">
         <v>311</v>
       </c>
@@ -5864,7 +5858,7 @@
         <v>313</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="192">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="192">
       <c r="A192" s="0" t="s">
         <v>314</v>
       </c>
@@ -5875,7 +5869,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="193">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="193">
       <c r="A193" s="0" t="s">
         <v>316</v>
       </c>
@@ -5886,7 +5880,7 @@
         <v>313</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="194">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="194">
       <c r="A194" s="0" t="s">
         <v>318</v>
       </c>
@@ -5897,7 +5891,7 @@
         <v>320</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="195">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="195">
       <c r="A195" s="0" t="s">
         <v>321</v>
       </c>
@@ -5908,7 +5902,7 @@
         <v>320</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="196">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="196">
       <c r="A196" s="0" t="s">
         <v>322</v>
       </c>
@@ -5919,7 +5913,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="197">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="197">
       <c r="A197" s="0" t="s">
         <v>324</v>
       </c>
@@ -5930,7 +5924,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="198">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="198">
       <c r="A198" s="0" t="s">
         <v>326</v>
       </c>
@@ -5941,7 +5935,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="199">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="199">
       <c r="A199" s="0" t="s">
         <v>328</v>
       </c>
@@ -5952,7 +5946,7 @@
         <v>299</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="200">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="200">
       <c r="A200" s="0" t="s">
         <v>330</v>
       </c>
@@ -5963,7 +5957,7 @@
         <v>332</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="201">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="201">
       <c r="A201" s="0" t="s">
         <v>333</v>
       </c>
@@ -5994,7 +5988,7 @@
         <v>338</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="17.45" outlineLevel="0" r="203">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="203">
       <c r="A203" s="0" t="s">
         <v>339</v>
       </c>
@@ -6014,7 +6008,7 @@
         <v>308</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="204">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="204">
       <c r="A204" s="0" t="s">
         <v>341</v>
       </c>
@@ -6028,7 +6022,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="205">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="205">
       <c r="A205" s="0" t="s">
         <v>344</v>
       </c>
@@ -6042,7 +6036,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="206">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="206">
       <c r="A206" s="0" t="s">
         <v>346</v>
       </c>
@@ -6056,7 +6050,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="207">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="207">
       <c r="A207" s="0" t="s">
         <v>348</v>
       </c>
@@ -6070,7 +6064,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="208">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="208">
       <c r="A208" s="0" t="s">
         <v>349</v>
       </c>
@@ -6084,7 +6078,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="209">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="209">
       <c r="A209" s="0" t="s">
         <v>351</v>
       </c>
@@ -6098,7 +6092,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="210">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="210">
       <c r="A210" s="0" t="s">
         <v>353</v>
       </c>
@@ -6112,7 +6106,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="211">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="211">
       <c r="A211" s="0" t="s">
         <v>355</v>
       </c>
@@ -6126,7 +6120,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="212">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="212">
       <c r="A212" s="0" t="s">
         <v>357</v>
       </c>
@@ -6140,7 +6134,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="213">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="213">
       <c r="A213" s="0" t="s">
         <v>358</v>
       </c>
@@ -6154,7 +6148,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="214">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="214">
       <c r="A214" s="0" t="s">
         <v>359</v>
       </c>
@@ -6168,7 +6162,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="215">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="215">
       <c r="A215" s="0" t="s">
         <v>360</v>
       </c>
@@ -6182,7 +6176,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="216">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="216">
       <c r="A216" s="0" t="s">
         <v>361</v>
       </c>
@@ -6196,7 +6190,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="217">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="217">
       <c r="A217" s="0" t="s">
         <v>362</v>
       </c>
@@ -6210,7 +6204,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="218">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="218">
       <c r="A218" s="0" t="s">
         <v>363</v>
       </c>
@@ -6224,7 +6218,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="219">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="219">
       <c r="A219" s="0" t="s">
         <v>364</v>
       </c>
@@ -6238,7 +6232,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="220">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="220">
       <c r="A220" s="0" t="s">
         <v>365</v>
       </c>
@@ -6252,7 +6246,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="221">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="221">
       <c r="A221" s="0" t="s">
         <v>366</v>
       </c>
@@ -6266,7 +6260,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="222">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="222">
       <c r="A222" s="0" t="s">
         <v>368</v>
       </c>
@@ -6280,7 +6274,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="223">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="223">
       <c r="A223" s="0" t="s">
         <v>369</v>
       </c>
@@ -6294,7 +6288,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="224">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="224">
       <c r="A224" s="0" t="s">
         <v>370</v>
       </c>
@@ -6308,7 +6302,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="225">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="225">
       <c r="A225" s="0" t="s">
         <v>371</v>
       </c>
@@ -6322,7 +6316,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="226">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="226">
       <c r="A226" s="0" t="s">
         <v>372</v>
       </c>
@@ -6336,7 +6330,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="227">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="227">
       <c r="A227" s="0" t="s">
         <v>373</v>
       </c>
@@ -6350,7 +6344,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="228">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="228">
       <c r="A228" s="0" t="s">
         <v>374</v>
       </c>
@@ -6364,7 +6358,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="229">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="229">
       <c r="A229" s="0" t="s">
         <v>375</v>
       </c>
@@ -6378,7 +6372,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="230">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="230">
       <c r="A230" s="0" t="s">
         <v>376</v>
       </c>
@@ -6392,7 +6386,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="231">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="231">
       <c r="A231" s="0" t="s">
         <v>378</v>
       </c>
@@ -6406,7 +6400,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="232">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="232">
       <c r="A232" s="0" t="s">
         <v>379</v>
       </c>
@@ -6420,7 +6414,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="233">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="233">
       <c r="A233" s="0" t="s">
         <v>380</v>
       </c>
@@ -6434,7 +6428,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="234">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="234">
       <c r="A234" s="0" t="s">
         <v>381</v>
       </c>
@@ -6448,7 +6442,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="235">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="235">
       <c r="A235" s="0" t="s">
         <v>382</v>
       </c>
@@ -6462,7 +6456,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="236">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="236">
       <c r="A236" s="0" t="s">
         <v>383</v>
       </c>
@@ -6476,7 +6470,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="237">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="237">
       <c r="A237" s="0" t="s">
         <v>384</v>
       </c>
@@ -6490,7 +6484,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="238">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="238">
       <c r="A238" s="0" t="s">
         <v>385</v>
       </c>
@@ -6504,7 +6498,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="239">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="239">
       <c r="A239" s="0" t="s">
         <v>386</v>
       </c>
@@ -6518,7 +6512,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="240">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="240">
       <c r="A240" s="0" t="s">
         <v>387</v>
       </c>
@@ -6532,7 +6526,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="241">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="241">
       <c r="A241" s="0" t="s">
         <v>388</v>
       </c>
@@ -6546,7 +6540,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="242">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="242">
       <c r="A242" s="0" t="s">
         <v>389</v>
       </c>
@@ -6560,7 +6554,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="243">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="243">
       <c r="A243" s="0" t="s">
         <v>390</v>
       </c>
@@ -6574,7 +6568,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="244">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="244">
       <c r="A244" s="0" t="s">
         <v>391</v>
       </c>
@@ -6588,7 +6582,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="245">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="245">
       <c r="A245" s="0" t="s">
         <v>392</v>
       </c>
@@ -6602,7 +6596,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="246">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="246">
       <c r="A246" s="0" t="s">
         <v>394</v>
       </c>
@@ -6616,7 +6610,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="247">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="247">
       <c r="A247" s="0" t="s">
         <v>395</v>
       </c>
@@ -6630,7 +6624,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="248">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="248">
       <c r="A248" s="0" t="s">
         <v>397</v>
       </c>
@@ -6644,7 +6638,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="249">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="249">
       <c r="A249" s="0" t="s">
         <v>398</v>
       </c>
@@ -6658,7 +6652,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="250">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="250">
       <c r="A250" s="0" t="s">
         <v>399</v>
       </c>
@@ -6672,7 +6666,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="251">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="251">
       <c r="A251" s="0" t="s">
         <v>400</v>
       </c>
@@ -6686,7 +6680,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="252">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="252">
       <c r="A252" s="0" t="s">
         <v>402</v>
       </c>
@@ -6700,7 +6694,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="253">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="253">
       <c r="A253" s="0" t="s">
         <v>403</v>
       </c>
@@ -6714,7 +6708,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="254">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="254">
       <c r="A254" s="0" t="s">
         <v>404</v>
       </c>
@@ -6728,7 +6722,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="255">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="255">
       <c r="A255" s="0" t="s">
         <v>405</v>
       </c>
@@ -6742,7 +6736,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="256">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="256">
       <c r="A256" s="0" t="s">
         <v>406</v>
       </c>
@@ -6756,7 +6750,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="257">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="257">
       <c r="A257" s="0" t="s">
         <v>407</v>
       </c>
@@ -6770,7 +6764,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="258">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="258">
       <c r="A258" s="0" t="s">
         <v>408</v>
       </c>
@@ -6784,7 +6778,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="259">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="259">
       <c r="A259" s="0" t="s">
         <v>409</v>
       </c>
@@ -6798,7 +6792,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="260">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="260">
       <c r="A260" s="0" t="s">
         <v>410</v>
       </c>
@@ -6812,7 +6806,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="261">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="261">
       <c r="A261" s="0" t="s">
         <v>411</v>
       </c>
@@ -6826,7 +6820,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="262">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="262">
       <c r="A262" s="0" t="s">
         <v>412</v>
       </c>
@@ -6840,7 +6834,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="263">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="263">
       <c r="A263" s="0" t="s">
         <v>413</v>
       </c>
@@ -6854,7 +6848,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="264">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="264">
       <c r="A264" s="0" t="s">
         <v>414</v>
       </c>
@@ -6868,7 +6862,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="265">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="265">
       <c r="A265" s="0" t="s">
         <v>415</v>
       </c>
@@ -6882,7 +6876,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="266">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="266">
       <c r="A266" s="0" t="s">
         <v>416</v>
       </c>
@@ -6896,7 +6890,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="267">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="267">
       <c r="A267" s="0" t="s">
         <v>417</v>
       </c>
@@ -6910,7 +6904,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="268">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="268">
       <c r="A268" s="0" t="s">
         <v>418</v>
       </c>
@@ -6924,7 +6918,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="269">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="269">
       <c r="A269" s="0" t="s">
         <v>419</v>
       </c>
@@ -6938,7 +6932,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="270">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="270">
       <c r="A270" s="0" t="s">
         <v>420</v>
       </c>
@@ -6952,7 +6946,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="271">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="271">
       <c r="A271" s="0" t="s">
         <v>421</v>
       </c>
@@ -6966,7 +6960,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="272">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="272">
       <c r="A272" s="0" t="s">
         <v>422</v>
       </c>
@@ -6980,7 +6974,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="273">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="273">
       <c r="A273" s="0" t="s">
         <v>423</v>
       </c>
@@ -6994,7 +6988,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="274">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="274">
       <c r="A274" s="0" t="s">
         <v>424</v>
       </c>
@@ -7008,7 +7002,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="275">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="275">
       <c r="A275" s="0" t="s">
         <v>425</v>
       </c>
@@ -7022,7 +7016,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="276">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="276">
       <c r="A276" s="0" t="s">
         <v>426</v>
       </c>
@@ -7036,7 +7030,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="277">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="277">
       <c r="A277" s="0" t="s">
         <v>427</v>
       </c>
@@ -7050,7 +7044,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="278">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="278">
       <c r="A278" s="0" t="s">
         <v>428</v>
       </c>
@@ -7064,7 +7058,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="279">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="279">
       <c r="A279" s="0" t="s">
         <v>429</v>
       </c>
@@ -7078,7 +7072,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="280">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="280">
       <c r="A280" s="0" t="s">
         <v>430</v>
       </c>
@@ -7092,7 +7086,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="281">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="281">
       <c r="A281" s="0" t="s">
         <v>431</v>
       </c>
@@ -7106,7 +7100,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="282">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="282">
       <c r="A282" s="0" t="s">
         <v>432</v>
       </c>
@@ -7120,7 +7114,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="283">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="283">
       <c r="A283" s="0" t="s">
         <v>433</v>
       </c>
@@ -7134,7 +7128,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="284">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="284">
       <c r="A284" s="0" t="s">
         <v>434</v>
       </c>
@@ -7148,7 +7142,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="285">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="285">
       <c r="A285" s="0" t="s">
         <v>435</v>
       </c>
@@ -7162,7 +7156,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="286">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="286">
       <c r="A286" s="0" t="s">
         <v>436</v>
       </c>
@@ -7176,7 +7170,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="287">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="287">
       <c r="A287" s="0" t="s">
         <v>437</v>
       </c>
@@ -7190,7 +7184,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="288">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="288">
       <c r="A288" s="0" t="s">
         <v>438</v>
       </c>
@@ -7204,7 +7198,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="289">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="289">
       <c r="A289" s="0" t="s">
         <v>439</v>
       </c>
@@ -7218,7 +7212,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="290">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="290">
       <c r="A290" s="0" t="s">
         <v>440</v>
       </c>
@@ -7232,7 +7226,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="291">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="291">
       <c r="A291" s="0" t="s">
         <v>441</v>
       </c>
@@ -7246,7 +7240,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="292">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="292">
       <c r="A292" s="0" t="s">
         <v>442</v>
       </c>
@@ -7260,7 +7254,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="293">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="293">
       <c r="A293" s="0" t="s">
         <v>443</v>
       </c>
@@ -7274,7 +7268,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="294">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="294">
       <c r="A294" s="0" t="s">
         <v>444</v>
       </c>
@@ -7288,7 +7282,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="295">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="295">
       <c r="A295" s="0" t="s">
         <v>445</v>
       </c>
@@ -7302,7 +7296,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="296">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="296">
       <c r="A296" s="0" t="s">
         <v>446</v>
       </c>
@@ -7316,7 +7310,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="297">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="297">
       <c r="A297" s="0" t="s">
         <v>448</v>
       </c>
@@ -7420,7 +7414,7 @@
         <v>453</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="303">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="303">
       <c r="A303" s="0" t="s">
         <v>458</v>
       </c>
@@ -7434,7 +7428,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="304">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="304">
       <c r="A304" s="0" t="s">
         <v>459</v>
       </c>
@@ -7448,7 +7442,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="305">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="305">
       <c r="A305" s="0" t="s">
         <v>460</v>
       </c>
@@ -7462,7 +7456,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="306">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="306">
       <c r="A306" s="0" t="s">
         <v>461</v>
       </c>
@@ -7476,7 +7470,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="307">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="307">
       <c r="A307" s="0" t="s">
         <v>462</v>
       </c>
@@ -7490,7 +7484,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="308">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="308">
       <c r="A308" s="0" t="s">
         <v>463</v>
       </c>
@@ -7504,7 +7498,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="309">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="309">
       <c r="A309" s="0" t="s">
         <v>464</v>
       </c>
@@ -7518,7 +7512,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="310">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="310">
       <c r="A310" s="0" t="s">
         <v>465</v>
       </c>
@@ -7532,7 +7526,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="311">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="311">
       <c r="A311" s="0" t="s">
         <v>466</v>
       </c>
@@ -7546,7 +7540,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="312">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="312">
       <c r="A312" s="0" t="s">
         <v>467</v>
       </c>
@@ -7560,7 +7554,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="313">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="313">
       <c r="A313" s="0" t="s">
         <v>468</v>
       </c>
@@ -7574,7 +7568,7 @@
         <v>343</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="314">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="314">
       <c r="A314" s="0" t="s">
         <v>469</v>
       </c>
@@ -8362,7 +8356,7 @@
         <v>523</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="354">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="354">
       <c r="A354" s="6" t="s">
         <v>569</v>
       </c>
@@ -8382,7 +8376,7 @@
         <v>573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="355">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="355">
       <c r="A355" s="6" t="s">
         <v>574</v>
       </c>
@@ -8462,7 +8456,7 @@
         <v>523</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="359">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="359">
       <c r="A359" s="6" t="s">
         <v>578</v>
       </c>
@@ -8482,7 +8476,7 @@
         <v>573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="360">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="360">
       <c r="A360" s="6" t="s">
         <v>579</v>
       </c>
@@ -8562,7 +8556,7 @@
         <v>523</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="364">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="364">
       <c r="A364" s="6" t="s">
         <v>583</v>
       </c>
@@ -8582,7 +8576,7 @@
         <v>573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="365">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="365">
       <c r="A365" s="6" t="s">
         <v>584</v>
       </c>
@@ -8662,7 +8656,7 @@
         <v>523</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="369">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="369">
       <c r="A369" s="6" t="s">
         <v>588</v>
       </c>
@@ -8682,7 +8676,7 @@
         <v>573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="370">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="370">
       <c r="A370" s="6" t="s">
         <v>589</v>
       </c>
@@ -8702,7 +8696,7 @@
         <v>573</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="371">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15.25" outlineLevel="0" r="371">
       <c r="A371" s="0" t="s">
         <v>590</v>
       </c>
@@ -8716,15 +8710,13 @@
         <v>593</v>
       </c>
       <c r="E371" s="14" t="s">
-        <v>594</v>
-      </c>
-      <c r="F371" s="9" t="s">
-        <v>595</v>
-      </c>
+        <v>591</v>
+      </c>
+      <c r="F371" s="9"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="16.4" outlineLevel="0" r="372">
       <c r="A372" s="0" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="B372" s="0" t="s">
         <v>476</v>
@@ -8742,312 +8734,312 @@
         <v>480</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="373">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="373">
       <c r="A373" s="0" t="s">
+        <v>595</v>
+      </c>
+      <c r="B373" s="5" t="s">
+        <v>596</v>
+      </c>
+      <c r="C373" s="5" t="s">
         <v>597</v>
       </c>
-      <c r="B373" s="5" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="374">
+      <c r="A374" s="0" t="s">
         <v>598</v>
       </c>
-      <c r="C373" s="5" t="s">
+      <c r="B374" s="5" t="s">
         <v>599</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="374">
-      <c r="A374" s="0" t="s">
+      <c r="C374" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="375">
+      <c r="A375" s="0" t="s">
         <v>600</v>
       </c>
-      <c r="B374" s="5" t="s">
+      <c r="B375" s="5" t="s">
         <v>601</v>
       </c>
-      <c r="C374" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="375">
-      <c r="A375" s="0" t="s">
+      <c r="C375" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="376">
+      <c r="A376" s="0" t="s">
         <v>602</v>
       </c>
-      <c r="B375" s="5" t="s">
+      <c r="B376" s="5" t="s">
         <v>603</v>
       </c>
-      <c r="C375" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="376">
-      <c r="A376" s="0" t="s">
+      <c r="C376" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="377">
+      <c r="A377" s="0" t="s">
         <v>604</v>
       </c>
-      <c r="B376" s="5" t="s">
+      <c r="B377" s="5" t="s">
         <v>605</v>
       </c>
-      <c r="C376" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="377">
-      <c r="A377" s="0" t="s">
+      <c r="C377" s="5" t="s">
         <v>606</v>
       </c>
-      <c r="B377" s="5" t="s">
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="378">
+      <c r="A378" s="0" t="s">
         <v>607</v>
       </c>
-      <c r="C377" s="5" t="s">
+      <c r="B378" s="5" t="s">
         <v>608</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="378">
-      <c r="A378" s="0" t="s">
+      <c r="C378" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="379">
+      <c r="A379" s="0" t="s">
         <v>609</v>
       </c>
-      <c r="B378" s="5" t="s">
+      <c r="B379" s="5" t="s">
         <v>610</v>
       </c>
-      <c r="C378" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="379">
-      <c r="A379" s="0" t="s">
+      <c r="C379" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="380">
+      <c r="A380" s="0" t="s">
         <v>611</v>
       </c>
-      <c r="B379" s="5" t="s">
+      <c r="B380" s="5" t="s">
         <v>612</v>
       </c>
-      <c r="C379" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="380">
-      <c r="A380" s="0" t="s">
+      <c r="C380" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="381">
+      <c r="A381" s="0" t="s">
         <v>613</v>
-      </c>
-      <c r="B380" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="C380" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="381">
-      <c r="A381" s="0" t="s">
-        <v>615</v>
       </c>
       <c r="B381" s="5" t="s">
         <v>334</v>
       </c>
       <c r="C381" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="382">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="382">
       <c r="A382" s="0" t="s">
+        <v>614</v>
+      </c>
+      <c r="B382" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="C382" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="383">
+      <c r="A383" s="0" t="s">
+        <v>615</v>
+      </c>
+      <c r="B383" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="C383" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="384">
+      <c r="A384" s="0" t="s">
         <v>616</v>
       </c>
-      <c r="B382" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="C382" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="383">
-      <c r="A383" s="0" t="s">
+      <c r="B384" s="5" t="s">
         <v>617</v>
       </c>
-      <c r="B383" s="5" t="s">
-        <v>614</v>
-      </c>
-      <c r="C383" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="384">
-      <c r="A384" s="0" t="s">
+      <c r="C384" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="385">
+      <c r="A385" s="0" t="s">
         <v>618</v>
       </c>
-      <c r="B384" s="5" t="s">
+      <c r="B385" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="C385" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="386">
+      <c r="A386" s="0" t="s">
         <v>619</v>
-      </c>
-      <c r="C384" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="385">
-      <c r="A385" s="0" t="s">
-        <v>620</v>
-      </c>
-      <c r="B385" s="5" t="s">
-        <v>619</v>
-      </c>
-      <c r="C385" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="386">
-      <c r="A386" s="0" t="s">
-        <v>621</v>
       </c>
       <c r="B386" s="5" t="s">
         <v>334</v>
       </c>
       <c r="C386" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="387">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="387">
       <c r="A387" s="0" t="s">
+        <v>620</v>
+      </c>
+      <c r="B387" s="5" t="s">
+        <v>621</v>
+      </c>
+      <c r="C387" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="388">
+      <c r="A388" s="0" t="s">
         <v>622</v>
-      </c>
-      <c r="B387" s="5" t="s">
-        <v>623</v>
-      </c>
-      <c r="C387" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="388">
-      <c r="A388" s="0" t="s">
-        <v>624</v>
       </c>
       <c r="B388" s="5" t="s">
         <v>319</v>
       </c>
       <c r="C388" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="389">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="389">
       <c r="A389" s="0" t="s">
+        <v>623</v>
+      </c>
+      <c r="B389" s="5" t="s">
+        <v>624</v>
+      </c>
+      <c r="C389" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="390">
+      <c r="A390" s="0" t="s">
         <v>625</v>
-      </c>
-      <c r="B389" s="5" t="s">
-        <v>626</v>
-      </c>
-      <c r="C389" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="390">
-      <c r="A390" s="0" t="s">
-        <v>627</v>
       </c>
       <c r="B390" s="5" t="s">
         <v>319</v>
       </c>
       <c r="C390" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="391">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="391">
       <c r="A391" s="0" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B391" s="5" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C391" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="392">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="392">
       <c r="A392" s="0" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="B392" s="5" t="s">
         <v>319</v>
       </c>
       <c r="C392" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="393">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="393">
       <c r="A393" s="0" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B393" s="5" t="s">
         <v>319</v>
       </c>
       <c r="C393" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="394">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="394">
       <c r="A394" s="0" t="s">
+        <v>629</v>
+      </c>
+      <c r="B394" s="5" t="s">
+        <v>617</v>
+      </c>
+      <c r="C394" s="5" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="395">
+      <c r="A395" s="0" t="s">
+        <v>630</v>
+      </c>
+      <c r="B395" s="5" t="s">
         <v>631</v>
       </c>
-      <c r="B394" s="5" t="s">
-        <v>619</v>
-      </c>
-      <c r="C394" s="5" t="s">
-        <v>608</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="395">
-      <c r="A395" s="0" t="s">
+      <c r="C395" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="396">
+      <c r="A396" s="0" t="s">
         <v>632</v>
       </c>
-      <c r="B395" s="5" t="s">
+      <c r="B396" s="5" t="s">
         <v>633</v>
       </c>
-      <c r="C395" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="396">
-      <c r="A396" s="0" t="s">
+      <c r="C396" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="397">
+      <c r="A397" s="0" t="s">
         <v>634</v>
       </c>
-      <c r="B396" s="5" t="s">
+      <c r="B397" s="5" t="s">
         <v>635</v>
       </c>
-      <c r="C396" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="397">
-      <c r="A397" s="0" t="s">
+      <c r="C397" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="398">
+      <c r="A398" s="0" t="s">
         <v>636</v>
       </c>
-      <c r="B397" s="5" t="s">
+      <c r="B398" s="5" t="s">
         <v>637</v>
       </c>
-      <c r="C397" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="398">
-      <c r="A398" s="0" t="s">
+      <c r="C398" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="399">
+      <c r="A399" s="0" t="s">
         <v>638</v>
       </c>
-      <c r="B398" s="5" t="s">
+      <c r="B399" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="C398" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="399">
-      <c r="A399" s="0" t="s">
+      <c r="C399" s="5" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="400">
+      <c r="A400" s="0" t="s">
         <v>640</v>
       </c>
-      <c r="B399" s="5" t="s">
+      <c r="B400" s="5" t="s">
         <v>641</v>
       </c>
-      <c r="C399" s="5" t="s">
-        <v>599</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="400">
-      <c r="A400" s="0" t="s">
-        <v>642</v>
-      </c>
-      <c r="B400" s="5" t="s">
-        <v>643</v>
-      </c>
       <c r="C400" s="5" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
   </sheetData>
@@ -9277,8 +9269,7 @@
     <hyperlink display="http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD" ref="F366" r:id="rId223"/>
     <hyperlink display="http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD" ref="F367" r:id="rId224"/>
     <hyperlink display="http://search.digikey.com/uk/en/products/NCP1529ASNT1G/NCP1529ASNT1GOSTR-ND/1792444" ref="F368" r:id="rId225"/>
-    <hyperlink display="http://uk.farnell.com/spansion/s25fl064k0smfi011/memory-flash-64m-3v-spi-8soic/dp/1861631?Ntt=S25FL064K" ref="F371" r:id="rId226"/>
-    <hyperlink display="http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD" ref="F372" r:id="rId227"/>
+    <hyperlink display="http://www.digikey.com/product-detail/en/NC7WZ17P6X/NC7WZ17P6XCT-ND/965707?cur=USD" ref="F372" r:id="rId226"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -9298,11 +9289,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="E189 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B371 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -9323,11 +9314,11 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="128" zoomScaleNormal="128" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="E189 A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="B371 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.67843137254902"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.71372549019608"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>